<commit_message>
Modified StableMotifs to PyStableMotifs and removed the local library, now it works with pip install. Modified the stable motif notebooks and ran the EMT heatmap code. Added the yED properties config file for plotting the succession diagrams.
</commit_message>
<xml_diff>
--- a/attractr_repertoire_and_stable_motif_analysis/EMT19_attractors.xlsx
+++ b/attractr_repertoire_and_stable_motif_analysis/EMT19_attractors.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -1764,6 +1764,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>